<commit_message>
Add FieldType that includes controlled term type
</commit_message>
<xml_diff>
--- a/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
+++ b/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B0DCA2-ADD0-C443-A6E5-DF6C920794AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B3CFD-8635-0F4E-A4FB-C7F7D52E3585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Repeat as necessary with incrementing numbers _3, _4 etc.
@@ -46,6 +47,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">Repeat as necessary with incrementing numbers _3, _4 etc.
@@ -60,6 +62,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Need to curated (Lucy)
@@ -72,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
   <si>
     <t>Field</t>
   </si>
@@ -226,6 +229,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> based on the FOA area</t>
@@ -302,27 +306,9 @@
     <t>creator_inst_name_1</t>
   </si>
   <si>
-    <t>e.g. Brown University</t>
-  </si>
-  <si>
     <t>creator_inst_id_1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">e.g. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://ror.org/05gq02987</t>
-    </r>
-  </si>
-  <si>
     <t>creator_inst_id_type_1</t>
   </si>
   <si>
@@ -353,21 +339,6 @@
     <t>creator_inst_id_2</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">e.g. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://ror.org/05gq02987</t>
-    </r>
-  </si>
-  <si>
     <t>creator_inst_id_type_2</t>
   </si>
   <si>
@@ -446,14 +417,17 @@
     <t>A sha256 digest of the data file</t>
   </si>
   <si>
-    <t>2007-04-05T12:30−02:00</t>
+    <t>Brown University</t>
+  </si>
+  <si>
+    <t>https://ror.org/05gq02987</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -521,6 +495,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -545,10 +534,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -575,8 +565,13 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1290,7 +1285,7 @@
         <v>55</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1319,10 +1314,10 @@
     </row>
     <row r="37" spans="1:26" ht="13">
       <c r="A37" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1351,10 +1346,10 @@
     </row>
     <row r="38" spans="1:26" ht="13">
       <c r="A38" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>24</v>
@@ -1390,7 +1385,7 @@
     </row>
     <row r="40" spans="1:26" ht="13">
       <c r="A40" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>4</v>
@@ -1422,7 +1417,7 @@
     </row>
     <row r="41" spans="1:26" ht="13">
       <c r="A41" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>6</v>
@@ -1454,7 +1449,7 @@
     </row>
     <row r="42" spans="1:26" ht="13">
       <c r="A42" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>9</v>
@@ -1486,7 +1481,7 @@
     </row>
     <row r="43" spans="1:26" ht="13">
       <c r="A43" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>12</v>
@@ -1518,7 +1513,7 @@
     </row>
     <row r="44" spans="1:26" ht="13">
       <c r="A44" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" s="11">
         <v>77816868</v>
@@ -1550,7 +1545,7 @@
     </row>
     <row r="45" spans="1:26" ht="13">
       <c r="A45" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>17</v>
@@ -1582,10 +1577,10 @@
     </row>
     <row r="46" spans="1:26" ht="13">
       <c r="A46" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="6"/>
@@ -1614,10 +1609,10 @@
     </row>
     <row r="47" spans="1:26" ht="13">
       <c r="A47" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="6"/>
@@ -1646,10 +1641,10 @@
     </row>
     <row r="48" spans="1:26" ht="13">
       <c r="A48" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>24</v>
@@ -1673,54 +1668,54 @@
     </row>
     <row r="50" spans="1:26" ht="13">
       <c r="A50" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:26" ht="13">
       <c r="A51" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:26" ht="13">
       <c r="A52" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:26" ht="13">
       <c r="A53" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:26" ht="13">
       <c r="A54" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:26" ht="13">
       <c r="A55" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:26" ht="13">
@@ -1729,11 +1724,11 @@
     </row>
     <row r="57" spans="1:26" ht="13">
       <c r="A57" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -1761,10 +1756,10 @@
     </row>
     <row r="58" spans="1:26" ht="13">
       <c r="A58" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:26" ht="13">
@@ -1772,40 +1767,40 @@
     </row>
     <row r="60" spans="1:26" ht="13">
       <c r="A60" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:26" ht="13">
       <c r="A61" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="13">
       <c r="A62" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="13">
       <c r="A63" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="B63" s="15">
+        <v>39177</v>
       </c>
     </row>
     <row r="64" spans="1:26" ht="13">
       <c r="A64" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="13">

</xml_diff>

<commit_message>
Refactor group data method
</commit_message>
<xml_diff>
--- a/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
+++ b/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5B3CFD-8635-0F4E-A4FB-C7F7D52E3585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8617887-CBEE-914F-8DE9-6AC43ABC12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="760" windowWidth="29100" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rad_014_328-01_META" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>Field</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>https://ror.org/05gq02987</t>
+  </si>
+  <si>
+    <t>https://radx.github.io/radx-metadata-specification-docs/radx-rad-mapping/#publication_url</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -567,6 +570,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -790,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1697,7 +1703,9 @@
       <c r="A53" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="16" t="s">
+        <v>95</v>
+      </c>
       <c r="C53" s="9" t="s">
         <v>76</v>
       </c>
@@ -4700,8 +4708,9 @@
     <hyperlink ref="C25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B37" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B47" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B53" r:id="rId4" location="publication_url" xr:uid="{DD4A8474-C6B2-5947-8771-F048FE6B5F23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extract common method from generators
</commit_message>
<xml_diff>
--- a/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
+++ b/src/test/resources/RADxRadMetadataTemplateSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycao77/bmir-radx/radx-rad-metadata-compiler/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8617887-CBEE-914F-8DE9-6AC43ABC12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B92E19-E5EA-A74B-924E-2DB5DF27B2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="760" windowWidth="29100" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="1840" windowWidth="29100" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rad_014_328-01_META" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
   <si>
     <t>Field</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>https://radx.github.io/radx-metadata-specification-docs/radx-rad-mapping/#publication_url</t>
+  </si>
+  <si>
+    <t>Contact PI</t>
+  </si>
+  <si>
+    <t>UEI</t>
   </si>
 </sst>
 </file>
@@ -796,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -908,6 +914,9 @@
     <row r="8" spans="1:26" ht="13">
       <c r="A8" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>20</v>
@@ -1650,7 +1659,7 @@
         <v>67</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>24</v>

</xml_diff>